<commit_message>
fim do processamento do arquivo
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Desktop\Pombo-Correio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38BD2154-A56C-4046-9E3B-44C1F74DB61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C397AE-FCC3-44BB-9892-82BAF3529A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12525" yWindow="2205" windowWidth="20025" windowHeight="10395" xr2:uid="{0A855E9A-822F-480E-80AB-FA166B8DDE69}"/>
+    <workbookView xWindow="3936" yWindow="12960" windowWidth="20028" windowHeight="10392" xr2:uid="{0A855E9A-822F-480E-80AB-FA166B8DDE69}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>estado</t>
   </si>
   <si>
-    <t xml:space="preserve">email </t>
-  </si>
-  <si>
     <t>nome</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,76 +464,76 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>